<commit_message>
update API Spec, API Detail
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_TranAnhDuy.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_TranAnhDuy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14085" tabRatio="818" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14085" tabRatio="818" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="180">
   <si>
     <t>No</t>
   </si>
@@ -423,9 +423,6 @@
   </si>
   <si>
     <t>version_id, rank_number, rank_type</t>
-  </si>
-  <si>
-    <t>Current date time as default value.</t>
   </si>
   <si>
     <t>Init version</t>
@@ -540,9 +537,6 @@
     <t>Birth Date</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -552,9 +546,6 @@
     <t>boss</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -567,9 +558,6 @@
     <t>DATETIME</t>
   </si>
   <si>
-    <t>VARCHAR(100)</t>
-  </si>
-  <si>
     <t>0:Female; 1:Male</t>
   </si>
   <si>
@@ -642,9 +630,6 @@
     <t>fk_comments_users1_idx</t>
   </si>
   <si>
-    <t>birthday</t>
-  </si>
-  <si>
     <t>birthdate</t>
   </si>
   <si>
@@ -667,12 +652,6 @@
   </si>
   <si>
     <t>duy.png</t>
-  </si>
-  <si>
-    <t>111D Lý Chính Thắng, Q.3</t>
-  </si>
-  <si>
-    <t>Tây Thạnh, Tân Phú</t>
   </si>
   <si>
     <t>vu@mulodo.com</t>
@@ -3251,7 +3230,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="247">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3666,6 +3645,156 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="14" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3792,162 +3921,6 @@
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="14" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="443">
@@ -5670,29 +5643,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="152"/>
-      <c r="P13" s="152"/>
-      <c r="Q13" s="152"/>
-      <c r="R13" s="152"/>
-      <c r="S13" s="152"/>
-      <c r="T13" s="152"/>
-      <c r="U13" s="152"/>
-      <c r="V13" s="152"/>
-      <c r="W13" s="152"/>
-      <c r="X13" s="152"/>
-      <c r="Y13" s="152"/>
-      <c r="Z13" s="152"/>
-      <c r="AA13" s="152"/>
-      <c r="AB13" s="152"/>
-      <c r="AC13" s="152"/>
-      <c r="AD13" s="152"/>
-      <c r="AE13" s="152"/>
-      <c r="AF13" s="152"/>
-      <c r="AG13" s="152"/>
-      <c r="AH13" s="152"/>
-      <c r="AI13" s="152"/>
-      <c r="AJ13" s="152"/>
-      <c r="AK13" s="152"/>
+      <c r="O13" s="202"/>
+      <c r="P13" s="202"/>
+      <c r="Q13" s="202"/>
+      <c r="R13" s="202"/>
+      <c r="S13" s="202"/>
+      <c r="T13" s="202"/>
+      <c r="U13" s="202"/>
+      <c r="V13" s="202"/>
+      <c r="W13" s="202"/>
+      <c r="X13" s="202"/>
+      <c r="Y13" s="202"/>
+      <c r="Z13" s="202"/>
+      <c r="AA13" s="202"/>
+      <c r="AB13" s="202"/>
+      <c r="AC13" s="202"/>
+      <c r="AD13" s="202"/>
+      <c r="AE13" s="202"/>
+      <c r="AF13" s="202"/>
+      <c r="AG13" s="202"/>
+      <c r="AH13" s="202"/>
+      <c r="AI13" s="202"/>
+      <c r="AJ13" s="202"/>
+      <c r="AK13" s="202"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5724,29 +5697,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="152"/>
-      <c r="P14" s="152"/>
-      <c r="Q14" s="152"/>
-      <c r="R14" s="152"/>
-      <c r="S14" s="152"/>
-      <c r="T14" s="152"/>
-      <c r="U14" s="152"/>
-      <c r="V14" s="152"/>
-      <c r="W14" s="152"/>
-      <c r="X14" s="152"/>
-      <c r="Y14" s="152"/>
-      <c r="Z14" s="152"/>
-      <c r="AA14" s="152"/>
-      <c r="AB14" s="152"/>
-      <c r="AC14" s="152"/>
-      <c r="AD14" s="152"/>
-      <c r="AE14" s="152"/>
-      <c r="AF14" s="152"/>
-      <c r="AG14" s="152"/>
-      <c r="AH14" s="152"/>
-      <c r="AI14" s="152"/>
-      <c r="AJ14" s="152"/>
-      <c r="AK14" s="152"/>
+      <c r="O14" s="202"/>
+      <c r="P14" s="202"/>
+      <c r="Q14" s="202"/>
+      <c r="R14" s="202"/>
+      <c r="S14" s="202"/>
+      <c r="T14" s="202"/>
+      <c r="U14" s="202"/>
+      <c r="V14" s="202"/>
+      <c r="W14" s="202"/>
+      <c r="X14" s="202"/>
+      <c r="Y14" s="202"/>
+      <c r="Z14" s="202"/>
+      <c r="AA14" s="202"/>
+      <c r="AB14" s="202"/>
+      <c r="AC14" s="202"/>
+      <c r="AD14" s="202"/>
+      <c r="AE14" s="202"/>
+      <c r="AF14" s="202"/>
+      <c r="AG14" s="202"/>
+      <c r="AH14" s="202"/>
+      <c r="AI14" s="202"/>
+      <c r="AJ14" s="202"/>
+      <c r="AK14" s="202"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5774,43 +5747,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="153" t="s">
-        <v>114</v>
-      </c>
-      <c r="L15" s="153"/>
-      <c r="M15" s="153"/>
-      <c r="N15" s="153"/>
-      <c r="O15" s="153"/>
-      <c r="P15" s="153"/>
-      <c r="Q15" s="153"/>
-      <c r="R15" s="153"/>
-      <c r="S15" s="153"/>
-      <c r="T15" s="153"/>
-      <c r="U15" s="153"/>
-      <c r="V15" s="153"/>
-      <c r="W15" s="153"/>
-      <c r="X15" s="153"/>
-      <c r="Y15" s="153"/>
-      <c r="Z15" s="153"/>
-      <c r="AA15" s="153"/>
-      <c r="AB15" s="153"/>
-      <c r="AC15" s="153"/>
-      <c r="AD15" s="153"/>
-      <c r="AE15" s="153"/>
-      <c r="AF15" s="153"/>
-      <c r="AG15" s="153"/>
-      <c r="AH15" s="153"/>
-      <c r="AI15" s="153"/>
-      <c r="AJ15" s="153"/>
-      <c r="AK15" s="153"/>
-      <c r="AL15" s="153"/>
-      <c r="AM15" s="153"/>
-      <c r="AN15" s="153"/>
-      <c r="AO15" s="153"/>
-      <c r="AP15" s="153"/>
-      <c r="AQ15" s="153"/>
-      <c r="AR15" s="153"/>
-      <c r="AS15" s="153"/>
+      <c r="K15" s="203" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="203"/>
+      <c r="M15" s="203"/>
+      <c r="N15" s="203"/>
+      <c r="O15" s="203"/>
+      <c r="P15" s="203"/>
+      <c r="Q15" s="203"/>
+      <c r="R15" s="203"/>
+      <c r="S15" s="203"/>
+      <c r="T15" s="203"/>
+      <c r="U15" s="203"/>
+      <c r="V15" s="203"/>
+      <c r="W15" s="203"/>
+      <c r="X15" s="203"/>
+      <c r="Y15" s="203"/>
+      <c r="Z15" s="203"/>
+      <c r="AA15" s="203"/>
+      <c r="AB15" s="203"/>
+      <c r="AC15" s="203"/>
+      <c r="AD15" s="203"/>
+      <c r="AE15" s="203"/>
+      <c r="AF15" s="203"/>
+      <c r="AG15" s="203"/>
+      <c r="AH15" s="203"/>
+      <c r="AI15" s="203"/>
+      <c r="AJ15" s="203"/>
+      <c r="AK15" s="203"/>
+      <c r="AL15" s="203"/>
+      <c r="AM15" s="203"/>
+      <c r="AN15" s="203"/>
+      <c r="AO15" s="203"/>
+      <c r="AP15" s="203"/>
+      <c r="AQ15" s="203"/>
+      <c r="AR15" s="203"/>
+      <c r="AS15" s="203"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5830,41 +5803,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
-      <c r="M16" s="153"/>
-      <c r="N16" s="153"/>
-      <c r="O16" s="153"/>
-      <c r="P16" s="153"/>
-      <c r="Q16" s="153"/>
-      <c r="R16" s="153"/>
-      <c r="S16" s="153"/>
-      <c r="T16" s="153"/>
-      <c r="U16" s="153"/>
-      <c r="V16" s="153"/>
-      <c r="W16" s="153"/>
-      <c r="X16" s="153"/>
-      <c r="Y16" s="153"/>
-      <c r="Z16" s="153"/>
-      <c r="AA16" s="153"/>
-      <c r="AB16" s="153"/>
-      <c r="AC16" s="153"/>
-      <c r="AD16" s="153"/>
-      <c r="AE16" s="153"/>
-      <c r="AF16" s="153"/>
-      <c r="AG16" s="153"/>
-      <c r="AH16" s="153"/>
-      <c r="AI16" s="153"/>
-      <c r="AJ16" s="153"/>
-      <c r="AK16" s="153"/>
-      <c r="AL16" s="153"/>
-      <c r="AM16" s="153"/>
-      <c r="AN16" s="153"/>
-      <c r="AO16" s="153"/>
-      <c r="AP16" s="153"/>
-      <c r="AQ16" s="153"/>
-      <c r="AR16" s="153"/>
-      <c r="AS16" s="153"/>
+      <c r="K16" s="203"/>
+      <c r="L16" s="203"/>
+      <c r="M16" s="203"/>
+      <c r="N16" s="203"/>
+      <c r="O16" s="203"/>
+      <c r="P16" s="203"/>
+      <c r="Q16" s="203"/>
+      <c r="R16" s="203"/>
+      <c r="S16" s="203"/>
+      <c r="T16" s="203"/>
+      <c r="U16" s="203"/>
+      <c r="V16" s="203"/>
+      <c r="W16" s="203"/>
+      <c r="X16" s="203"/>
+      <c r="Y16" s="203"/>
+      <c r="Z16" s="203"/>
+      <c r="AA16" s="203"/>
+      <c r="AB16" s="203"/>
+      <c r="AC16" s="203"/>
+      <c r="AD16" s="203"/>
+      <c r="AE16" s="203"/>
+      <c r="AF16" s="203"/>
+      <c r="AG16" s="203"/>
+      <c r="AH16" s="203"/>
+      <c r="AI16" s="203"/>
+      <c r="AJ16" s="203"/>
+      <c r="AK16" s="203"/>
+      <c r="AL16" s="203"/>
+      <c r="AM16" s="203"/>
+      <c r="AN16" s="203"/>
+      <c r="AO16" s="203"/>
+      <c r="AP16" s="203"/>
+      <c r="AQ16" s="203"/>
+      <c r="AR16" s="203"/>
+      <c r="AS16" s="203"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6453,14 +6426,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="154">
+      <c r="AN27" s="204">
         <v>41651</v>
       </c>
-      <c r="AO27" s="154"/>
-      <c r="AP27" s="154"/>
-      <c r="AQ27" s="154"/>
-      <c r="AR27" s="154"/>
-      <c r="AS27" s="154"/>
+      <c r="AO27" s="204"/>
+      <c r="AP27" s="204"/>
+      <c r="AQ27" s="204"/>
+      <c r="AR27" s="204"/>
+      <c r="AS27" s="204"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -6963,11 +6936,11 @@
         <v>41651</v>
       </c>
       <c r="C3" s="114" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="94"/>
       <c r="E3" s="95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="96"/>
     </row>
@@ -7219,11 +7192,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" thickBot="1">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="205" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -7241,10 +7214,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="122" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="135" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15">
@@ -7253,10 +7226,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="123" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="136" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15">
@@ -7265,10 +7238,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="136" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -7484,10 +7457,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView topLeftCell="L6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="K6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -7505,129 +7478,128 @@
     <col min="13" max="13" width="12.42578125" style="13" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" style="13" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="17" style="197" customWidth="1"/>
-    <col min="17" max="17" width="30.140625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="23.42578125" style="197" customWidth="1"/>
-    <col min="19" max="19" width="17" style="13" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="13"/>
+    <col min="16" max="16" width="17" style="154" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" style="154" customWidth="1"/>
+    <col min="18" max="18" width="17" style="13" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="12.75" thickBot="1">
+    <row r="1" spans="1:18" ht="12.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.25">
+    <row r="2" spans="1:18" ht="14.25">
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="177" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="182"/>
+      <c r="C2" s="227" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="232"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="177" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="178"/>
-    </row>
-    <row r="3" spans="1:19" ht="14.25">
+      <c r="F2" s="227" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="228"/>
+    </row>
+    <row r="3" spans="1:18" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="233"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="179" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="180"/>
-    </row>
-    <row r="4" spans="1:19" ht="14.25">
+      <c r="F3" s="229" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="230"/>
+    </row>
+    <row r="4" spans="1:18" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="181" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="183"/>
+      <c r="C4" s="231" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="233"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="181"/>
-      <c r="G4" s="180"/>
-    </row>
-    <row r="5" spans="1:19" ht="24">
+      <c r="F4" s="231"/>
+      <c r="G4" s="230"/>
+    </row>
+    <row r="5" spans="1:18" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="181" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="183"/>
+      <c r="C5" s="231" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="233"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="180"/>
-    </row>
-    <row r="6" spans="1:19" ht="24">
+      <c r="F5" s="231"/>
+      <c r="G5" s="230"/>
+    </row>
+    <row r="6" spans="1:18" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="181" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="183"/>
+      <c r="C6" s="231" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="233"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="180"/>
-    </row>
-    <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="165" t="s">
+      <c r="F6" s="231"/>
+      <c r="G6" s="230"/>
+    </row>
+    <row r="7" spans="1:18" ht="14.25">
+      <c r="B7" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="167"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="B9" s="171"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
-    </row>
-    <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="172"/>
-      <c r="C10" s="173"/>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
-    </row>
-    <row r="12" spans="1:19" ht="12.75" thickBot="1">
+      <c r="C7" s="216"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="216"/>
+      <c r="G7" s="217"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="B8" s="218"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="220"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="B9" s="221"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="220"/>
+    </row>
+    <row r="10" spans="1:18" ht="12.75" thickBot="1">
+      <c r="B10" s="222"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
+    </row>
+    <row r="12" spans="1:18" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="30" t="s">
         <v>0</v>
       </c>
@@ -7649,49 +7621,46 @@
       <c r="G13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="201" t="s">
+      <c r="I13" s="158" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="159" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="J13" s="202" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" s="202" t="s">
-        <v>112</v>
-      </c>
-      <c r="L13" s="202" t="s">
+      <c r="L13" s="159" t="s">
+        <v>131</v>
+      </c>
+      <c r="M13" s="159" t="s">
         <v>132</v>
       </c>
-      <c r="M13" s="202" t="s">
-        <v>133</v>
-      </c>
-      <c r="N13" s="202" t="s">
+      <c r="N13" s="159" t="s">
+        <v>129</v>
+      </c>
+      <c r="O13" s="160" t="s">
         <v>130</v>
       </c>
-      <c r="O13" s="203" t="s">
-        <v>131</v>
-      </c>
-      <c r="P13" s="202" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q13" s="203" t="s">
-        <v>139</v>
-      </c>
-      <c r="R13" s="202" t="s">
-        <v>140</v>
-      </c>
-      <c r="S13" s="204" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15">
+      <c r="P13" s="159" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q13" s="159" t="s">
+        <v>137</v>
+      </c>
+      <c r="R13" s="161" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15">
       <c r="A14" s="69">
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" s="65" t="s">
         <v>53</v>
@@ -7704,109 +7673,103 @@
         <v>50</v>
       </c>
       <c r="H14" s="87"/>
-      <c r="I14" s="205">
+      <c r="I14" s="162">
         <v>1</v>
       </c>
-      <c r="J14" s="206" t="s">
+      <c r="J14" s="163" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="K14" s="206" t="s">
-        <v>108</v>
-      </c>
-      <c r="L14" s="207" t="s">
+      <c r="L14" s="164" t="s">
+        <v>166</v>
+      </c>
+      <c r="M14" s="165" t="s">
+        <v>167</v>
+      </c>
+      <c r="N14" s="164" t="s">
         <v>171</v>
       </c>
-      <c r="M14" s="208" t="s">
-        <v>172</v>
-      </c>
-      <c r="N14" s="207" t="s">
-        <v>176</v>
-      </c>
-      <c r="O14" s="209">
+      <c r="O14" s="166">
         <v>1</v>
       </c>
-      <c r="P14" s="210">
+      <c r="P14" s="167">
         <v>31321</v>
       </c>
-      <c r="Q14" s="211" t="s">
-        <v>178</v>
-      </c>
-      <c r="R14" s="212" t="s">
-        <v>180</v>
-      </c>
-      <c r="S14" s="213">
+      <c r="Q14" s="168" t="s">
+        <v>173</v>
+      </c>
+      <c r="R14" s="169">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1">
       <c r="A15" s="59">
         <f>A14+1</f>
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="65" t="s">
-        <v>104</v>
-      </c>
       <c r="D15" s="65" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H15" s="87"/>
-      <c r="I15" s="214">
+      <c r="I15" s="170">
         <v>2</v>
       </c>
-      <c r="J15" s="215" t="s">
-        <v>173</v>
-      </c>
-      <c r="K15" s="216" t="s">
-        <v>110</v>
-      </c>
-      <c r="L15" s="215" t="s">
+      <c r="J15" s="171" t="s">
+        <v>168</v>
+      </c>
+      <c r="K15" s="172" t="s">
+        <v>109</v>
+      </c>
+      <c r="L15" s="171" t="s">
+        <v>169</v>
+      </c>
+      <c r="M15" s="173" t="s">
+        <v>170</v>
+      </c>
+      <c r="N15" s="171" t="s">
+        <v>172</v>
+      </c>
+      <c r="O15" s="174">
+        <v>1</v>
+      </c>
+      <c r="P15" s="175">
+        <v>32874</v>
+      </c>
+      <c r="Q15" s="176" t="s">
         <v>174</v>
       </c>
-      <c r="M15" s="217" t="s">
-        <v>175</v>
-      </c>
-      <c r="N15" s="215" t="s">
-        <v>177</v>
-      </c>
-      <c r="O15" s="218">
-        <v>1</v>
-      </c>
-      <c r="P15" s="219">
-        <v>32874</v>
-      </c>
-      <c r="Q15" s="220" t="s">
-        <v>179</v>
-      </c>
-      <c r="R15" s="221" t="s">
-        <v>181</v>
-      </c>
-      <c r="S15" s="222">
+      <c r="R15" s="177">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16" s="59">
-        <f t="shared" ref="A16:A23" si="0">A15+1</f>
+        <f t="shared" ref="A16:A21" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -7821,13 +7784,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
@@ -7841,13 +7804,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
@@ -7861,13 +7824,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
@@ -7881,13 +7844,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
@@ -7896,7 +7859,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="106" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -7905,13 +7868,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E21" s="66" t="s">
         <v>3</v>
@@ -7921,181 +7884,158 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="59">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E22" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="67"/>
-      <c r="G22" s="106" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="59">
-        <f t="shared" si="0"/>
+      <c r="G22" s="106"/>
+    </row>
+    <row r="23" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A23" s="70">
         <v>10</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="130" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="131" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="65" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="E23" s="66" t="s">
+      <c r="D23" s="131" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="67"/>
-      <c r="G23" s="106"/>
-    </row>
-    <row r="24" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A24" s="70">
-        <v>11</v>
-      </c>
-      <c r="B24" s="130" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="131" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="131" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" s="132" t="s">
+      <c r="F23" s="134" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="133" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="24">
+      <c r="A26" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="213" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="214"/>
+      <c r="E26" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.25">
+      <c r="A27" s="14">
+        <v>1</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="225" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="226"/>
+      <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="134" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="133" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="24">
-      <c r="A27" s="29" t="s">
+      <c r="F27" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="12.95" customHeight="1">
+      <c r="A28" s="57">
+        <v>2</v>
+      </c>
+      <c r="B28" s="51"/>
+      <c r="C28" s="211"/>
+      <c r="D28" s="212"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="53"/>
+    </row>
+    <row r="29" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
+      <c r="A29" s="56">
+        <v>3</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="209"/>
+      <c r="D29" s="210"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="55"/>
+    </row>
+    <row r="31" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" thickBot="1">
+      <c r="A32" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="163" t="s">
+      <c r="B32" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="164"/>
-      <c r="E27" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="14.25">
-      <c r="A28" s="14">
-        <v>1</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="175" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="176"/>
-      <c r="E28" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" ht="12.95" customHeight="1">
-      <c r="A29" s="57">
-        <v>2</v>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="161"/>
-      <c r="D29" s="162"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53"/>
-    </row>
-    <row r="30" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A30" s="56">
-        <v>3</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="159"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="55"/>
-    </row>
-    <row r="32" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A32" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1">
-      <c r="A33" s="36" t="s">
+      <c r="D32" s="207"/>
+      <c r="E32" s="206" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="208"/>
+      <c r="G32" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="12.75" thickBot="1">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" thickBot="1">
+      <c r="A35" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="156" t="s">
+      <c r="C35" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="157"/>
-      <c r="E33" s="156" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33" s="158"/>
-      <c r="G33" s="38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="12.75" thickBot="1">
-      <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1">
-      <c r="A36" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="156" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="157"/>
-      <c r="E36" s="156" t="s">
+      <c r="D35" s="207"/>
+      <c r="E35" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="158"/>
-      <c r="G36" s="38" t="s">
+      <c r="F35" s="208"/>
+      <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
     </row>
@@ -8111,21 +8051,21 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="R14" r:id="rId1"/>
-    <hyperlink ref="R15" r:id="rId2"/>
+    <hyperlink ref="Q14" r:id="rId1"/>
+    <hyperlink ref="Q15" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
@@ -8148,7 +8088,7 @@
   </sheetPr>
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="H8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="L8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -8165,7 +8105,7 @@
     <col min="12" max="12" width="12.7109375" style="13" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" style="13" customWidth="1"/>
     <col min="14" max="15" width="19.28515625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="17" style="197" customWidth="1"/>
+    <col min="16" max="16" width="17" style="154" customWidth="1"/>
     <col min="17" max="17" width="17" style="13" customWidth="1"/>
     <col min="18" max="18" width="15.42578125" style="13" customWidth="1"/>
     <col min="19" max="16384" width="8.85546875" style="13"/>
@@ -8180,110 +8120,110 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="177" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="182"/>
+      <c r="C2" s="227" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="232"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="177" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="178"/>
+      <c r="F2" s="227" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="228"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="233"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="179" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="180"/>
+      <c r="F3" s="229" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="230"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="181" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="183"/>
+      <c r="C4" s="231" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="233"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="181"/>
-      <c r="G4" s="180"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="230"/>
     </row>
     <row r="5" spans="1:19" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="181" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="183"/>
+      <c r="C5" s="231" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="233"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="180"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="230"/>
     </row>
     <row r="6" spans="1:19" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="181" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="183"/>
+      <c r="C6" s="231" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="233"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="180"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="230"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="167"/>
+      <c r="C7" s="216"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="216"/>
+      <c r="G7" s="217"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="218"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="220"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="171"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="221"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="220"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="172"/>
-      <c r="C10" s="173"/>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
+      <c r="B10" s="222"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -8308,40 +8248,40 @@
       <c r="G13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="201" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="224" t="s">
+      <c r="I13" s="158" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="179" t="s">
+        <v>144</v>
+      </c>
+      <c r="K13" s="179" t="s">
+        <v>146</v>
+      </c>
+      <c r="L13" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="K13" s="224" t="s">
-        <v>150</v>
-      </c>
-      <c r="L13" s="224" t="s">
+      <c r="M13" s="179" t="s">
+        <v>175</v>
+      </c>
+      <c r="N13" s="179" t="s">
         <v>152</v>
       </c>
-      <c r="M13" s="224" t="s">
-        <v>182</v>
-      </c>
-      <c r="N13" s="224" t="s">
-        <v>156</v>
-      </c>
-      <c r="O13" s="225" t="s">
-        <v>158</v>
+      <c r="O13" s="180" t="s">
+        <v>154</v>
       </c>
       <c r="Q13" s="128"/>
       <c r="R13" s="128"/>
-      <c r="S13" s="195"/>
+      <c r="S13" s="152"/>
     </row>
     <row r="14" spans="1:19" ht="15">
       <c r="A14" s="69">
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" s="65" t="s">
         <v>53</v>
@@ -8354,25 +8294,25 @@
         <v>50</v>
       </c>
       <c r="H14" s="87"/>
-      <c r="I14" s="205">
+      <c r="I14" s="162">
         <v>1</v>
       </c>
-      <c r="J14" s="206" t="s">
+      <c r="J14" s="163" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="K14" s="206" t="s">
-        <v>108</v>
-      </c>
-      <c r="L14" s="226">
+      <c r="L14" s="181">
         <v>41306</v>
       </c>
-      <c r="M14" s="227">
+      <c r="M14" s="182">
         <v>41770</v>
       </c>
-      <c r="N14" s="206">
+      <c r="N14" s="163">
         <v>0</v>
       </c>
-      <c r="O14" s="228">
+      <c r="O14" s="183">
         <v>1</v>
       </c>
       <c r="Q14" s="127"/>
@@ -8384,13 +8324,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -8398,25 +8338,25 @@
       <c r="F15" s="67"/>
       <c r="G15" s="107"/>
       <c r="H15" s="87"/>
-      <c r="I15" s="214">
+      <c r="I15" s="170">
         <v>2</v>
       </c>
-      <c r="J15" s="216" t="s">
+      <c r="J15" s="172" t="s">
+        <v>108</v>
+      </c>
+      <c r="K15" s="172" t="s">
         <v>109</v>
       </c>
-      <c r="K15" s="216" t="s">
-        <v>110</v>
-      </c>
-      <c r="L15" s="229">
+      <c r="L15" s="184">
         <v>41963</v>
       </c>
-      <c r="M15" s="230">
+      <c r="M15" s="185">
         <v>42063</v>
       </c>
-      <c r="N15" s="216">
+      <c r="N15" s="172">
         <v>0</v>
       </c>
-      <c r="O15" s="231">
+      <c r="O15" s="186">
         <v>2</v>
       </c>
       <c r="Q15" s="127"/>
@@ -8428,13 +8368,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -8452,10 +8392,10 @@
         <v>41</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E17" s="66"/>
       <c r="F17" s="67"/>
@@ -8470,10 +8410,10 @@
         <v>42</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E18" s="66"/>
       <c r="F18" s="67"/>
@@ -8485,20 +8425,20 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="66"/>
       <c r="F19" s="137" t="s">
         <v>4</v>
       </c>
       <c r="G19" s="106" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" thickBot="1">
@@ -8506,10 +8446,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="130" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="131" t="s">
         <v>154</v>
-      </c>
-      <c r="C20" s="131" t="s">
-        <v>158</v>
       </c>
       <c r="D20" s="131" t="s">
         <v>53</v>
@@ -8530,10 +8470,10 @@
       <c r="B23" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="163" t="s">
+      <c r="C23" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="164"/>
+      <c r="D23" s="214"/>
       <c r="E23" s="34" t="s">
         <v>33</v>
       </c>
@@ -8551,10 +8491,10 @@
       <c r="B24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="175" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="176"/>
+      <c r="C24" s="225" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="226"/>
       <c r="E24" s="46" t="s">
         <v>3</v>
       </c>
@@ -8568,8 +8508,8 @@
         <v>2</v>
       </c>
       <c r="B25" s="51"/>
-      <c r="C25" s="161"/>
-      <c r="D25" s="162"/>
+      <c r="C25" s="211"/>
+      <c r="D25" s="212"/>
       <c r="E25" s="52"/>
       <c r="F25" s="52"/>
       <c r="G25" s="53"/>
@@ -8579,8 +8519,8 @@
         <v>3</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="160"/>
+      <c r="C26" s="209"/>
+      <c r="D26" s="210"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58"/>
       <c r="G26" s="55"/>
@@ -8597,14 +8537,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="156" t="s">
+      <c r="C29" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="157"/>
-      <c r="E29" s="156" t="s">
+      <c r="D29" s="207"/>
+      <c r="E29" s="206" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="158"/>
+      <c r="F29" s="208"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -8614,18 +8554,18 @@
         <v>1</v>
       </c>
       <c r="B30" s="140" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="184" t="s">
-        <v>158</v>
-      </c>
-      <c r="D30" s="184"/>
-      <c r="E30" s="184" t="s">
-        <v>122</v>
-      </c>
-      <c r="F30" s="184"/>
+        <v>155</v>
+      </c>
+      <c r="C30" s="234" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="234"/>
+      <c r="E30" s="234" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="234"/>
       <c r="G30" s="141" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" thickBot="1">
@@ -8640,14 +8580,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="156" t="s">
+      <c r="C32" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="157"/>
-      <c r="E32" s="156" t="s">
+      <c r="D32" s="207"/>
+      <c r="E32" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="158"/>
+      <c r="F32" s="208"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -8693,7 +8633,7 @@
   </sheetPr>
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="K11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -8710,9 +8650,9 @@
     <col min="11" max="11" width="30" style="13" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="13" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="196" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" style="197" customWidth="1"/>
-    <col min="16" max="16" width="17" style="197" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="153" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" style="154" customWidth="1"/>
+    <col min="16" max="16" width="17" style="154" customWidth="1"/>
     <col min="17" max="17" width="17" style="13" customWidth="1"/>
     <col min="18" max="18" width="15.42578125" style="13" customWidth="1"/>
     <col min="19" max="16384" width="8.85546875" style="13"/>
@@ -8727,110 +8667,110 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="177" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="182"/>
+      <c r="C2" s="227" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="232"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="177" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="178"/>
+      <c r="F2" s="227" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="228"/>
     </row>
     <row r="3" spans="1:26" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="233"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="179" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="180"/>
+      <c r="F3" s="229" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="230"/>
     </row>
     <row r="4" spans="1:26" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="181" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="183"/>
+      <c r="C4" s="231" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="233"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="181"/>
-      <c r="G4" s="180"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="230"/>
     </row>
     <row r="5" spans="1:26" ht="14.25">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="181" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="183"/>
+      <c r="C5" s="231" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="233"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="180"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="230"/>
     </row>
     <row r="6" spans="1:26" ht="14.25">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="181" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" s="183"/>
+      <c r="C6" s="231" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="233"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="180"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="230"/>
     </row>
     <row r="7" spans="1:26" ht="14.25">
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="167"/>
+      <c r="C7" s="216"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="216"/>
+      <c r="G7" s="217"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="218"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="220"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="B9" s="171"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="221"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="220"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" thickBot="1">
-      <c r="B10" s="172"/>
-      <c r="C10" s="173"/>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
+      <c r="B10" s="222"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
     </row>
     <row r="12" spans="1:26" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="142" customFormat="1" ht="12.75" thickTop="1">
@@ -8855,34 +8795,34 @@
       <c r="G13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="223"/>
-      <c r="I13" s="234" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="235" t="s">
+      <c r="H13" s="178"/>
+      <c r="I13" s="189" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="190" t="s">
+        <v>144</v>
+      </c>
+      <c r="K13" s="190" t="s">
+        <v>146</v>
+      </c>
+      <c r="L13" s="190" t="s">
         <v>148</v>
       </c>
-      <c r="K13" s="235" t="s">
-        <v>150</v>
-      </c>
-      <c r="L13" s="235" t="s">
+      <c r="M13" s="190" t="s">
+        <v>175</v>
+      </c>
+      <c r="N13" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="M13" s="235" t="s">
-        <v>182</v>
-      </c>
-      <c r="N13" s="235" t="s">
-        <v>156</v>
-      </c>
-      <c r="O13" s="236" t="s">
-        <v>166</v>
-      </c>
-      <c r="P13" s="237" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q13" s="233"/>
-      <c r="R13" s="233"/>
-      <c r="S13" s="233"/>
+      <c r="O13" s="191" t="s">
+        <v>162</v>
+      </c>
+      <c r="P13" s="192" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q13" s="188"/>
+      <c r="R13" s="188"/>
+      <c r="S13" s="188"/>
       <c r="T13" s="143"/>
       <c r="U13" s="143"/>
       <c r="V13" s="143"/>
@@ -8896,10 +8836,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" s="65" t="s">
         <v>53</v>
@@ -8911,29 +8851,29 @@
       <c r="G14" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="232"/>
-      <c r="I14" s="238">
+      <c r="H14" s="187"/>
+      <c r="I14" s="193">
         <v>1</v>
       </c>
-      <c r="J14" s="207" t="s">
-        <v>183</v>
-      </c>
-      <c r="K14" s="207" t="s">
-        <v>185</v>
-      </c>
-      <c r="L14" s="226">
+      <c r="J14" s="164" t="s">
+        <v>176</v>
+      </c>
+      <c r="K14" s="164" t="s">
+        <v>178</v>
+      </c>
+      <c r="L14" s="181">
         <v>40901</v>
       </c>
-      <c r="M14" s="226">
+      <c r="M14" s="181">
         <v>41455</v>
       </c>
-      <c r="N14" s="239">
+      <c r="N14" s="194">
         <v>0</v>
       </c>
-      <c r="O14" s="209">
+      <c r="O14" s="166">
         <v>1</v>
       </c>
-      <c r="P14" s="240">
+      <c r="P14" s="195">
         <v>2</v>
       </c>
       <c r="Q14" s="144"/>
@@ -8945,42 +8885,42 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="67"/>
       <c r="G15" s="107"/>
-      <c r="H15" s="232"/>
-      <c r="I15" s="241">
+      <c r="H15" s="187"/>
+      <c r="I15" s="196">
         <v>2</v>
       </c>
-      <c r="J15" s="242" t="s">
-        <v>184</v>
-      </c>
-      <c r="K15" s="242" t="s">
-        <v>186</v>
-      </c>
-      <c r="L15" s="246">
+      <c r="J15" s="197" t="s">
+        <v>177</v>
+      </c>
+      <c r="K15" s="197" t="s">
+        <v>179</v>
+      </c>
+      <c r="L15" s="201">
         <v>40493</v>
       </c>
-      <c r="M15" s="246">
+      <c r="M15" s="201">
         <v>41255</v>
       </c>
-      <c r="N15" s="243">
+      <c r="N15" s="198">
         <v>0</v>
       </c>
-      <c r="O15" s="244">
+      <c r="O15" s="199">
         <v>2</v>
       </c>
-      <c r="P15" s="245">
+      <c r="P15" s="200">
         <v>1</v>
       </c>
       <c r="Q15" s="144"/>
@@ -8992,23 +8932,23 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117"/>
-      <c r="H16" s="232"/>
-      <c r="N16" s="200"/>
-      <c r="O16" s="199"/>
-      <c r="P16" s="199"/>
+      <c r="H16" s="187"/>
+      <c r="N16" s="157"/>
+      <c r="O16" s="156"/>
+      <c r="P16" s="156"/>
     </row>
     <row r="17" spans="1:26" s="143" customFormat="1">
       <c r="A17" s="59">
@@ -9016,21 +8956,21 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E17" s="66"/>
       <c r="F17" s="67"/>
       <c r="G17" s="117"/>
-      <c r="H17" s="223"/>
-      <c r="N17" s="200"/>
-      <c r="O17" s="199"/>
-      <c r="P17" s="199"/>
+      <c r="H17" s="178"/>
+      <c r="N17" s="157"/>
+      <c r="O17" s="156"/>
+      <c r="P17" s="156"/>
     </row>
     <row r="18" spans="1:26" s="143" customFormat="1">
       <c r="A18" s="59">
@@ -9040,19 +8980,19 @@
       <c r="B18" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="198" t="s">
-        <v>182</v>
+      <c r="C18" s="155" t="s">
+        <v>175</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E18" s="66"/>
       <c r="F18" s="67"/>
       <c r="G18" s="106"/>
-      <c r="H18" s="223"/>
-      <c r="N18" s="200"/>
-      <c r="O18" s="199"/>
-      <c r="P18" s="199"/>
+      <c r="H18" s="178"/>
+      <c r="N18" s="157"/>
+      <c r="O18" s="156"/>
+      <c r="P18" s="156"/>
     </row>
     <row r="19" spans="1:26" s="143" customFormat="1">
       <c r="A19" s="59">
@@ -9060,25 +9000,25 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C19" s="145" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="66"/>
       <c r="F19" s="137" t="s">
         <v>4</v>
       </c>
       <c r="G19" s="106" t="s">
-        <v>165</v>
-      </c>
-      <c r="H19" s="223"/>
-      <c r="N19" s="200"/>
-      <c r="O19" s="199"/>
-      <c r="P19" s="199"/>
+        <v>161</v>
+      </c>
+      <c r="H19" s="178"/>
+      <c r="N19" s="157"/>
+      <c r="O19" s="156"/>
+      <c r="P19" s="156"/>
     </row>
     <row r="20" spans="1:26" s="143" customFormat="1">
       <c r="A20" s="59">
@@ -9086,10 +9026,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D20" s="129" t="s">
         <v>53</v>
@@ -9097,10 +9037,10 @@
       <c r="E20" s="66"/>
       <c r="F20" s="67"/>
       <c r="G20" s="106"/>
-      <c r="H20" s="223"/>
-      <c r="N20" s="200"/>
-      <c r="O20" s="199"/>
-      <c r="P20" s="199"/>
+      <c r="H20" s="178"/>
+      <c r="N20" s="157"/>
+      <c r="O20" s="156"/>
+      <c r="P20" s="156"/>
     </row>
     <row r="21" spans="1:26" s="150" customFormat="1" ht="12.75" thickBot="1">
       <c r="A21" s="70">
@@ -9108,10 +9048,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="146" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="68" t="s">
         <v>154</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>158</v>
       </c>
       <c r="D21" s="68" t="s">
         <v>53</v>
@@ -9119,15 +9059,15 @@
       <c r="E21" s="147"/>
       <c r="F21" s="148"/>
       <c r="G21" s="149"/>
-      <c r="H21" s="223"/>
+      <c r="H21" s="178"/>
       <c r="I21" s="143"/>
       <c r="J21" s="143"/>
       <c r="K21" s="143"/>
       <c r="L21" s="143"/>
       <c r="M21" s="143"/>
-      <c r="N21" s="200"/>
-      <c r="O21" s="199"/>
-      <c r="P21" s="199"/>
+      <c r="N21" s="157"/>
+      <c r="O21" s="156"/>
+      <c r="P21" s="156"/>
       <c r="Q21" s="143"/>
       <c r="R21" s="143"/>
       <c r="S21" s="143"/>
@@ -9151,10 +9091,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="163" t="s">
+      <c r="C24" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="164"/>
+      <c r="D24" s="214"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -9172,10 +9112,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="175" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="176"/>
+      <c r="C25" s="225" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="226"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -9189,8 +9129,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="51"/>
-      <c r="C26" s="161"/>
-      <c r="D26" s="162"/>
+      <c r="C26" s="211"/>
+      <c r="D26" s="212"/>
       <c r="E26" s="52"/>
       <c r="F26" s="52"/>
       <c r="G26" s="53"/>
@@ -9200,8 +9140,8 @@
         <v>3</v>
       </c>
       <c r="B27" s="54"/>
-      <c r="C27" s="159"/>
-      <c r="D27" s="160"/>
+      <c r="C27" s="209"/>
+      <c r="D27" s="210"/>
       <c r="E27" s="58"/>
       <c r="F27" s="58"/>
       <c r="G27" s="55"/>
@@ -9218,14 +9158,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="156" t="s">
+      <c r="C30" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="157"/>
-      <c r="E30" s="156" t="s">
+      <c r="D30" s="207"/>
+      <c r="E30" s="206" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="158"/>
+      <c r="F30" s="208"/>
       <c r="G30" s="38" t="s">
         <v>38</v>
       </c>
@@ -9235,18 +9175,18 @@
         <v>1</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" s="185" t="s">
-        <v>166</v>
-      </c>
-      <c r="D31" s="185"/>
-      <c r="E31" s="185" t="s">
-        <v>123</v>
-      </c>
-      <c r="F31" s="185"/>
+        <v>163</v>
+      </c>
+      <c r="C31" s="235" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="235"/>
+      <c r="E31" s="235" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="235"/>
       <c r="G31" s="138" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:26">
@@ -9254,18 +9194,18 @@
         <v>2</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" s="186" t="s">
-        <v>158</v>
-      </c>
-      <c r="D32" s="186"/>
-      <c r="E32" s="186" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="186"/>
+        <v>164</v>
+      </c>
+      <c r="C32" s="236" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="236"/>
+      <c r="E32" s="236" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="236"/>
       <c r="G32" s="138" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -9286,14 +9226,14 @@
       <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="156" t="s">
+      <c r="C35" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="157"/>
-      <c r="E35" s="156" t="s">
+      <c r="D35" s="207"/>
+      <c r="E35" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="158"/>
+      <c r="F35" s="208"/>
       <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
@@ -9365,103 +9305,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="177" t="s">
+      <c r="C2" s="227" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="182"/>
+      <c r="D2" s="232"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="177" t="s">
+      <c r="F2" s="227" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="178"/>
+      <c r="G2" s="228"/>
     </row>
     <row r="3" spans="1:11" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="233"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="181" t="s">
+      <c r="F3" s="231" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="180"/>
+      <c r="G3" s="230"/>
     </row>
     <row r="4" spans="1:11" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="181" t="s">
+      <c r="C4" s="231" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="183"/>
+      <c r="D4" s="233"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="181"/>
-      <c r="G4" s="180"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="230"/>
     </row>
     <row r="5" spans="1:11" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="181" t="s">
+      <c r="C5" s="231" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="183"/>
+      <c r="D5" s="233"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="180"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="230"/>
     </row>
     <row r="6" spans="1:11" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="231" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="183"/>
+      <c r="D6" s="233"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="180"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="230"/>
     </row>
     <row r="7" spans="1:11" ht="14.25">
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="167"/>
+      <c r="C7" s="216"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="216"/>
+      <c r="G7" s="217"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="218"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="220"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="171"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="221"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="220"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" thickBot="1">
-      <c r="B10" s="172"/>
-      <c r="C10" s="173"/>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
+      <c r="B10" s="222"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9683,10 +9623,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="163" t="s">
+      <c r="C24" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="164"/>
+      <c r="D24" s="214"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -9704,10 +9644,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="175" t="s">
+      <c r="C25" s="225" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="176"/>
+      <c r="D25" s="226"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -9721,10 +9661,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="189" t="s">
+      <c r="C26" s="239" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="190"/>
+      <c r="D26" s="240"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -9743,14 +9683,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="156" t="s">
+      <c r="C29" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="157"/>
-      <c r="E29" s="156" t="s">
+      <c r="D29" s="207"/>
+      <c r="E29" s="206" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="158"/>
+      <c r="F29" s="208"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -9767,14 +9707,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="156" t="s">
+      <c r="C32" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="157"/>
-      <c r="E32" s="156" t="s">
+      <c r="D32" s="207"/>
+      <c r="E32" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="158"/>
+      <c r="F32" s="208"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -9784,14 +9724,14 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="187" t="s">
+      <c r="C33" s="237" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="188"/>
-      <c r="E33" s="189" t="s">
+      <c r="D33" s="238"/>
+      <c r="E33" s="239" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="190"/>
+      <c r="F33" s="240"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
@@ -9866,105 +9806,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="177" t="s">
+      <c r="C2" s="227" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="182"/>
+      <c r="D2" s="232"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="177" t="s">
+      <c r="F2" s="227" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="178"/>
+      <c r="G2" s="228"/>
     </row>
     <row r="3" spans="1:7" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="233"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="181" t="s">
+      <c r="F3" s="231" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="180"/>
+      <c r="G3" s="230"/>
     </row>
     <row r="4" spans="1:7" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="181" t="s">
+      <c r="C4" s="231" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="183"/>
+      <c r="D4" s="233"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="181"/>
-      <c r="G4" s="180"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="230"/>
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="181" t="s">
+      <c r="C5" s="231" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="183"/>
+      <c r="D5" s="233"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="180"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="230"/>
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="231" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="183"/>
+      <c r="D6" s="233"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="180"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="230"/>
     </row>
     <row r="7" spans="1:7" ht="14.25">
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="167"/>
+      <c r="C7" s="216"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="216"/>
+      <c r="G7" s="217"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="168" t="s">
+      <c r="B8" s="218" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="220"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="171"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="221"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="220"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" thickBot="1">
-      <c r="B10" s="172"/>
-      <c r="C10" s="173"/>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
+      <c r="B10" s="222"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
     </row>
     <row r="12" spans="1:7" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10069,10 +10009,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="163" t="s">
+      <c r="C19" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="164"/>
+      <c r="D19" s="214"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -10090,10 +10030,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="175" t="s">
+      <c r="C20" s="225" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="176"/>
+      <c r="D20" s="226"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -10107,10 +10047,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="187" t="s">
+      <c r="C21" s="237" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="188"/>
+      <c r="D21" s="238"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -10129,14 +10069,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="156" t="s">
+      <c r="C24" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="157"/>
-      <c r="E24" s="156" t="s">
+      <c r="D24" s="207"/>
+      <c r="E24" s="206" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="158"/>
+      <c r="F24" s="208"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -10153,14 +10093,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="156" t="s">
+      <c r="C27" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="157"/>
-      <c r="E27" s="156" t="s">
+      <c r="D27" s="207"/>
+      <c r="E27" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="158"/>
+      <c r="F27" s="208"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -10170,10 +10110,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="187"/>
-      <c r="D28" s="188"/>
-      <c r="E28" s="189"/>
-      <c r="F28" s="190"/>
+      <c r="C28" s="237"/>
+      <c r="D28" s="238"/>
+      <c r="E28" s="239"/>
+      <c r="F28" s="240"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
@@ -10246,103 +10186,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="177" t="s">
+      <c r="C2" s="227" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="182"/>
+      <c r="D2" s="232"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="193" t="s">
+      <c r="F2" s="243" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="194"/>
+      <c r="G2" s="244"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="233"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="179" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="180"/>
+      <c r="F3" s="229" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="230"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="181" t="s">
+      <c r="C4" s="231" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="183"/>
+      <c r="D4" s="233"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="181"/>
-      <c r="G4" s="180"/>
+      <c r="F4" s="231"/>
+      <c r="G4" s="230"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="181" t="s">
+      <c r="C5" s="231" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="183"/>
+      <c r="D5" s="233"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="180"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="230"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="183"/>
+      <c r="D6" s="233"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="180"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="230"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="167"/>
+      <c r="C7" s="216"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="216"/>
+      <c r="G7" s="217"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="218"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="220"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="171"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="221"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="220"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="172"/>
-      <c r="C10" s="173"/>
-      <c r="D10" s="173"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
+      <c r="B10" s="222"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -10558,10 +10498,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="163" t="s">
+      <c r="C21" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="164"/>
+      <c r="D21" s="214"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -10585,10 +10525,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="175" t="s">
+      <c r="C22" s="225" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="176"/>
+      <c r="D22" s="226"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -10608,10 +10548,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="161" t="s">
+      <c r="C23" s="211" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="162"/>
+      <c r="D23" s="212"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -10629,10 +10569,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="187" t="s">
+      <c r="C24" s="237" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="188"/>
+      <c r="D24" s="238"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -10671,14 +10611,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="156" t="s">
+      <c r="C27" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="157"/>
-      <c r="E27" s="156" t="s">
+      <c r="D27" s="207"/>
+      <c r="E27" s="206" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="158"/>
+      <c r="F27" s="208"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -10715,14 +10655,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="156" t="s">
+      <c r="C30" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="157"/>
-      <c r="E30" s="156" t="s">
+      <c r="D30" s="207"/>
+      <c r="E30" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="158"/>
+      <c r="F30" s="208"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -10738,14 +10678,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="175" t="s">
+      <c r="C31" s="225" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="176"/>
-      <c r="E31" s="161" t="s">
+      <c r="D31" s="226"/>
+      <c r="E31" s="211" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="162"/>
+      <c r="F31" s="212"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -10761,14 +10701,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="191" t="s">
+      <c r="C32" s="241" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="192"/>
-      <c r="E32" s="189" t="s">
+      <c r="D32" s="242"/>
+      <c r="E32" s="239" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="190"/>
+      <c r="F32" s="240"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>

</xml_diff>